<commit_message>
#fix: - product:    + import thiếu 2 trường highlight & chương trình đặc biệt    + hiển thị thông tin chi tiết sản phẩm thiếu url3, url4
</commit_message>
<xml_diff>
--- a/admin/src/assets/importProductTemplateCamera.xlsx
+++ b/admin/src/assets/importProductTemplateCamera.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C909E8CA-10CB-462E-97DD-C0AE4E9ACD0A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Category</t>
   </si>
@@ -110,12 +111,18 @@
   </si>
   <si>
     <t>Tính năng</t>
+  </si>
+  <si>
+    <t>Highlight</t>
+  </si>
+  <si>
+    <t>Chương trình đặc biệt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -499,36 +506,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.85546875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="14.140625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="18.28515625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="2"/>
+    <col min="12" max="12" width="19.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="24.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.88671875" style="2" customWidth="1"/>
+    <col min="18" max="18" width="16.5546875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="17.109375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="14.109375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="18.33203125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="15.44140625" style="2" customWidth="1"/>
+    <col min="23" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -572,25 +581,31 @@
         <v>11</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>

</xml_diff>